<commit_message>
detailed locations of Siberian birds
</commit_message>
<xml_diff>
--- a/metadata/GW_locations_LatLong_2023.xlsx
+++ b/metadata/GW_locations_LatLong_2023.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darrenirwin/Dropbox/Darren's current work/GW manuscript 2022_2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darrenirwin/Documents/Github_repos_MacBookPro/GW_genomics_2023/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFFDA5D-3358-024B-A1F5-88FC98F54BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{099B033B-FD97-5143-8BA4-25F5AAA0F294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="500" windowWidth="28340" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="520" yWindow="3000" windowWidth="28340" windowHeight="18360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="GW location LatLong.txt" sheetId="1" r:id="rId1"/>
+    <sheet name="GW_locations_LatLong_2023" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="85">
   <si>
     <t>YK</t>
   </si>
@@ -97,15 +97,9 @@
     <t>plumbeitarsus</t>
   </si>
   <si>
-    <t>KK</t>
-  </si>
-  <si>
     <t>ST_vi</t>
   </si>
   <si>
-    <t>KK_vi</t>
-  </si>
-  <si>
     <t>Beijing</t>
   </si>
   <si>
@@ -127,15 +121,9 @@
     <t>Stolbi</t>
   </si>
   <si>
-    <t>Krasnoyarski_Krai</t>
-  </si>
-  <si>
     <t>Teletsk</t>
   </si>
   <si>
-    <t>Krasnoyarski_Krai_vi</t>
-  </si>
-  <si>
     <t>Manali</t>
   </si>
   <si>
@@ -211,9 +199,6 @@
     <t>Langtang</t>
   </si>
   <si>
-    <t>Ala Archa</t>
-  </si>
-  <si>
     <t>Abakan</t>
   </si>
   <si>
@@ -242,6 +227,54 @@
   </si>
   <si>
     <t>Yekaterinburg</t>
+  </si>
+  <si>
+    <t>VB</t>
+  </si>
+  <si>
+    <t>Divnogorsk</t>
+  </si>
+  <si>
+    <t>DV</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>Manskoe_Belogorie</t>
+  </si>
+  <si>
+    <t>Verkh_Biryusa</t>
+  </si>
+  <si>
+    <t>Predivinsk</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>Gongga</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>Ala_Archa</t>
+  </si>
+  <si>
+    <t>Divnogorsk_vir</t>
+  </si>
+  <si>
+    <t>DV_vi</t>
+  </si>
+  <si>
+    <t>Stolbi_vir</t>
+  </si>
+  <si>
+    <t>VB_vi</t>
+  </si>
+  <si>
+    <t>Verkh_Biryusa_vir</t>
   </si>
 </sst>
 </file>
@@ -288,13 +321,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -691,32 +722,32 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2">
         <v>56.8</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2">
         <v>60.6</v>
       </c>
       <c r="E2" t="s">
@@ -724,16 +755,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3">
         <v>52</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3">
         <v>89.5</v>
       </c>
       <c r="E3" t="s">
@@ -741,16 +772,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>51.7</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4">
         <v>87.6</v>
       </c>
       <c r="E4" t="s">
@@ -758,101 +789,101 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="A5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5">
         <v>55.9</v>
       </c>
-      <c r="D5" s="4">
-        <v>92.6</v>
+      <c r="D5">
+        <v>92</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="4">
-        <v>55.9</v>
-      </c>
-      <c r="D6" s="4">
-        <v>92.6</v>
+      <c r="A6" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6">
+        <v>56</v>
+      </c>
+      <c r="D6">
+        <v>92.4</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>55.9</v>
+      </c>
+      <c r="D7">
+        <v>92.6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C8">
         <v>41</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D8">
         <v>42</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="4" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C9">
         <v>42.54</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D9">
         <v>74.5</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="4">
-        <v>34.594000000000001</v>
-      </c>
-      <c r="D9" s="4">
-        <v>73.465999999999994</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10">
         <v>34.884</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10">
         <v>73.691000000000003</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -860,373 +891,373 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="4">
-        <v>33.991</v>
-      </c>
-      <c r="D11" s="4">
-        <v>75.242999999999995</v>
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11">
+        <v>34.594000000000001</v>
+      </c>
+      <c r="D11">
+        <v>73.465999999999994</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="4">
-        <v>32.973999999999997</v>
-      </c>
-      <c r="D12" s="4">
-        <v>76.221999999999994</v>
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12">
+        <v>33.991</v>
+      </c>
+      <c r="D12">
+        <v>75.242999999999995</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="4">
-        <v>33.106000000000002</v>
-      </c>
-      <c r="D13" s="4">
-        <v>76.409000000000006</v>
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13">
+        <v>32.973999999999997</v>
+      </c>
+      <c r="D13">
+        <v>76.221999999999994</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="4">
-        <v>32.828000000000003</v>
-      </c>
-      <c r="D14" s="4">
-        <v>76.45</v>
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>33.106000000000002</v>
+      </c>
+      <c r="D14">
+        <v>76.409000000000006</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="4">
-        <v>33.134</v>
-      </c>
-      <c r="D15" s="4">
-        <v>76.454999999999998</v>
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15">
+        <v>32.828000000000003</v>
+      </c>
+      <c r="D15">
+        <v>76.45</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="4">
-        <v>32.771000000000001</v>
-      </c>
-      <c r="D16" s="4">
-        <v>76.471999999999994</v>
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16">
+        <v>33.134</v>
+      </c>
+      <c r="D16">
+        <v>76.454999999999998</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="4">
-        <v>32.868000000000002</v>
-      </c>
-      <c r="D17" s="4">
-        <v>76.855000000000004</v>
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>32.771000000000001</v>
+      </c>
+      <c r="D17">
+        <v>76.471999999999994</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="4">
-        <v>32.728000000000002</v>
-      </c>
-      <c r="D18" s="4">
-        <v>76.859399999999994</v>
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>32.868000000000002</v>
+      </c>
+      <c r="D18">
+        <v>76.855000000000004</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="4">
-        <v>32.508000000000003</v>
-      </c>
-      <c r="D19" s="4">
-        <v>76.980999999999995</v>
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19">
+        <v>32.728000000000002</v>
+      </c>
+      <c r="D19">
+        <v>76.859399999999994</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="4">
-        <v>32.237000000000002</v>
-      </c>
-      <c r="D20" s="4">
-        <v>77.13</v>
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>32.508000000000003</v>
+      </c>
+      <c r="D20">
+        <v>76.980999999999995</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="4">
-        <v>32.377000000000002</v>
-      </c>
-      <c r="D21" s="3">
-        <v>77.281000000000006</v>
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>32.237000000000002</v>
+      </c>
+      <c r="D21">
+        <v>77.13</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22">
+        <v>32.377000000000002</v>
+      </c>
+      <c r="D22" s="2">
+        <v>77.281000000000006</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>28.25</v>
+      </c>
+      <c r="D23">
+        <v>85.5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24">
+        <v>29.5</v>
+      </c>
+      <c r="D24">
+        <v>102</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25">
+        <v>29.5</v>
+      </c>
+      <c r="D25">
+        <v>103.3</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="4">
-        <v>28.25</v>
-      </c>
-      <c r="D22" s="4">
-        <v>85.5</v>
-      </c>
-      <c r="E22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="4">
-        <v>29.5</v>
-      </c>
-      <c r="D23" s="4">
-        <v>103.3</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>102</v>
+      </c>
+      <c r="E26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="4">
-        <v>37</v>
-      </c>
-      <c r="D24" s="4">
-        <v>102</v>
-      </c>
-      <c r="E24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="3">
         <v>40</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D27">
         <v>115.5</v>
-      </c>
-      <c r="E25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="4">
-        <v>51.9</v>
-      </c>
-      <c r="D26" s="4">
-        <v>104.9</v>
-      </c>
-      <c r="E26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="4">
-        <v>51.9</v>
-      </c>
-      <c r="D27" s="4">
-        <v>102.5</v>
       </c>
       <c r="E27" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="4">
-        <v>51.1</v>
-      </c>
-      <c r="D28" s="4">
-        <v>95.5</v>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>51.9</v>
+      </c>
+      <c r="D28">
+        <v>104.9</v>
       </c>
       <c r="E28" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="4">
-        <v>51.3</v>
-      </c>
-      <c r="D29" s="4">
-        <v>92</v>
+      <c r="A29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29">
+        <v>51.9</v>
+      </c>
+      <c r="D29">
+        <v>102.5</v>
       </c>
       <c r="E29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="4">
-        <v>55.9</v>
-      </c>
-      <c r="D30" s="4">
-        <v>92.6</v>
+      <c r="A30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30">
+        <v>51.1</v>
+      </c>
+      <c r="D30">
+        <v>95.5</v>
       </c>
       <c r="E30" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" s="4">
-        <v>55.9</v>
-      </c>
-      <c r="D31" s="4">
-        <v>92.6</v>
+      <c r="A31" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31">
+        <v>51.3</v>
+      </c>
+      <c r="D31">
+        <v>92</v>
       </c>
       <c r="E31" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32">
         <v>51.9</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32">
         <v>94.1</v>
       </c>
       <c r="E32" t="s">
@@ -1234,19 +1265,104 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33">
+        <v>54.7</v>
+      </c>
+      <c r="D33">
+        <v>94</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34">
+        <v>55.9</v>
+      </c>
+      <c r="D34">
+        <v>92</v>
+      </c>
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
         <v>70</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35">
+        <v>56</v>
+      </c>
+      <c r="D35">
+        <v>92.4</v>
+      </c>
+      <c r="E35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>55.9</v>
+      </c>
+      <c r="D36">
+        <v>92.6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37">
+        <v>57.1</v>
+      </c>
+      <c r="D37">
+        <v>93.5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A38" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C38">
         <v>55.7</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D38">
         <v>91</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E38" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>